<commit_message>
Updated to have all variants requested
</commit_message>
<xml_diff>
--- a/doc/Vehicle_Matrix.xlsx
+++ b/doc/Vehicle_Matrix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\P072220\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p072220\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F44F6F4-9497-4EDF-AF34-1CC135808B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B6BCCF-9C79-47EE-B4F3-23DD05B5E961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9C560BEE-8399-4795-B8CB-4D83758CC15A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="31320" windowHeight="15630" xr2:uid="{9C560BEE-8399-4795-B8CB-4D83758CC15A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -781,47 +781,137 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -829,118 +919,28 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1265,7 +1265,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1305,178 +1305,178 @@
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="22" t="s">
+      <c r="B2" s="53" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="22">
+      <c r="D2" s="12">
         <v>2022</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="22">
-        <v>4</v>
-      </c>
-      <c r="G2" s="23" t="s">
+      <c r="F2" s="12">
+        <v>4</v>
+      </c>
+      <c r="G2" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="35" t="s">
         <v>2</v>
       </c>
       <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="52"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="24" t="s">
+      <c r="A3" s="51"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="14">
         <v>2019</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="24">
-        <v>4</v>
-      </c>
-      <c r="G3" s="25" t="s">
+      <c r="F3" s="14">
+        <v>4</v>
+      </c>
+      <c r="G3" s="15" t="s">
         <v>69</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="8"/>
-      <c r="J3" s="16"/>
+      <c r="J3" s="33"/>
       <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="52"/>
-      <c r="B4" s="60"/>
-      <c r="C4" s="57" t="s">
+      <c r="A4" s="51"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="57">
+      <c r="D4" s="28">
         <v>2020</v>
       </c>
-      <c r="E4" s="57" t="s">
+      <c r="E4" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="57">
-        <v>4</v>
-      </c>
-      <c r="G4" s="58" t="s">
+      <c r="F4" s="28">
+        <v>4</v>
+      </c>
+      <c r="G4" s="29" t="s">
         <v>19</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="8"/>
-      <c r="J4" s="16"/>
+      <c r="J4" s="33"/>
       <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="52"/>
-      <c r="B5" s="12" t="s">
+      <c r="A5" s="51"/>
+      <c r="B5" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="12">
         <v>2017</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="22">
-        <v>4</v>
-      </c>
-      <c r="G5" s="23" t="s">
+      <c r="F5" s="12">
+        <v>4</v>
+      </c>
+      <c r="G5" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="8"/>
-      <c r="J5" s="16" t="s">
+      <c r="J5" s="33" t="s">
         <v>3</v>
       </c>
       <c r="K5" s="9"/>
     </row>
     <row r="6" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="52"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="24" t="s">
+      <c r="A6" s="51"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="14">
         <v>2018</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="24">
-        <v>2</v>
-      </c>
-      <c r="G6" s="25" t="s">
+      <c r="F6" s="14">
+        <v>2</v>
+      </c>
+      <c r="G6" s="15" t="s">
         <v>69</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="8"/>
-      <c r="J6" s="16"/>
+      <c r="J6" s="33"/>
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="52"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="28" t="s">
+      <c r="A7" s="51"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="28">
+      <c r="D7" s="16">
         <v>2017</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="28">
-        <v>4</v>
-      </c>
-      <c r="G7" s="29" t="s">
+      <c r="F7" s="16">
+        <v>4</v>
+      </c>
+      <c r="G7" s="17" t="s">
         <v>19</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="8"/>
-      <c r="J7" s="16"/>
+      <c r="J7" s="33"/>
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="52"/>
-      <c r="B8" s="61" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="26" t="s">
+      <c r="A8" s="51"/>
+      <c r="B8" s="65" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="53">
+      <c r="D8" s="26">
         <v>2019</v>
       </c>
-      <c r="E8" s="53" t="s">
+      <c r="E8" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="53">
-        <v>2</v>
-      </c>
-      <c r="G8" s="54" t="s">
+      <c r="F8" s="26">
+        <v>2</v>
+      </c>
+      <c r="G8" s="27" t="s">
         <v>70</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="8"/>
-      <c r="J8" s="16" t="s">
+      <c r="J8" s="33" t="s">
         <v>4</v>
       </c>
       <c r="K8" s="9" t="s">
@@ -1484,78 +1484,78 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="52"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="24">
+      <c r="A9" s="51"/>
+      <c r="B9" s="54"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="14">
         <v>2017</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F9" s="24">
-        <v>2</v>
-      </c>
-      <c r="G9" s="25" t="s">
+      <c r="F9" s="14">
+        <v>2</v>
+      </c>
+      <c r="G9" s="15" t="s">
         <v>26</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="8"/>
-      <c r="J9" s="16"/>
+      <c r="J9" s="33"/>
       <c r="K9" s="9" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="56"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="28">
+      <c r="A10" s="52"/>
+      <c r="B10" s="55"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="16">
         <v>2016</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="28">
-        <v>2</v>
-      </c>
-      <c r="G10" s="29" t="s">
+      <c r="F10" s="16">
+        <v>2</v>
+      </c>
+      <c r="G10" s="17" t="s">
         <v>19</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="10"/>
-      <c r="J10" s="17"/>
+      <c r="J10" s="34"/>
       <c r="K10" s="11" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="30" t="s">
+      <c r="B11" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="30">
+      <c r="D11" s="18">
         <v>2014</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="30">
-        <v>2</v>
-      </c>
-      <c r="G11" s="31" t="s">
+      <c r="F11" s="18">
+        <v>2</v>
+      </c>
+      <c r="G11" s="19" t="s">
         <v>21</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="J11" s="15" t="s">
+      <c r="J11" s="35" t="s">
         <v>2</v>
       </c>
       <c r="K11" s="7" t="s">
@@ -1563,151 +1563,151 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="48"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="32" t="s">
+      <c r="A12" s="62"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="32">
+      <c r="D12" s="20">
         <v>2021</v>
       </c>
-      <c r="E12" s="32" t="s">
+      <c r="E12" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="32">
-        <v>4</v>
-      </c>
-      <c r="G12" s="33" t="s">
+      <c r="F12" s="20">
+        <v>4</v>
+      </c>
+      <c r="G12" s="21" t="s">
         <v>26</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="8"/>
-      <c r="J12" s="16"/>
+      <c r="J12" s="33"/>
       <c r="K12" s="9" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="48"/>
-      <c r="B13" s="62"/>
-      <c r="C13" s="63" t="s">
+      <c r="A13" s="62"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="63">
+      <c r="D13" s="30">
         <v>2017</v>
       </c>
-      <c r="E13" s="63" t="s">
+      <c r="E13" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="63">
-        <v>4</v>
-      </c>
-      <c r="G13" s="64" t="s">
+      <c r="F13" s="30">
+        <v>4</v>
+      </c>
+      <c r="G13" s="31" t="s">
         <v>19</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="8"/>
-      <c r="J13" s="16"/>
+      <c r="J13" s="33"/>
       <c r="K13" s="9" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="48"/>
-      <c r="B14" s="19" t="s">
+      <c r="A14" s="62"/>
+      <c r="B14" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="30">
+      <c r="D14" s="18">
         <v>2015</v>
       </c>
-      <c r="E14" s="30" t="s">
+      <c r="E14" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="30">
-        <v>4</v>
-      </c>
-      <c r="G14" s="31" t="s">
+      <c r="F14" s="18">
+        <v>4</v>
+      </c>
+      <c r="G14" s="19" t="s">
         <v>21</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="8"/>
-      <c r="J14" s="16" t="s">
+      <c r="J14" s="33" t="s">
         <v>3</v>
       </c>
       <c r="K14" s="9"/>
     </row>
     <row r="15" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="48"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="32" t="s">
+      <c r="A15" s="62"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="32">
+      <c r="D15" s="20">
         <v>2011</v>
       </c>
-      <c r="E15" s="32" t="s">
+      <c r="E15" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="32">
-        <v>2</v>
-      </c>
-      <c r="G15" s="33" t="s">
+      <c r="F15" s="20">
+        <v>2</v>
+      </c>
+      <c r="G15" s="21" t="s">
         <v>26</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="8"/>
-      <c r="J15" s="16"/>
+      <c r="J15" s="33"/>
       <c r="K15" s="9"/>
     </row>
     <row r="16" spans="1:11" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="48"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="36" t="s">
+      <c r="A16" s="62"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="36">
+      <c r="D16" s="22">
         <v>2016</v>
       </c>
-      <c r="E16" s="36" t="s">
+      <c r="E16" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="36">
-        <v>4</v>
-      </c>
-      <c r="G16" s="37" t="s">
+      <c r="F16" s="22">
+        <v>4</v>
+      </c>
+      <c r="G16" s="23" t="s">
         <v>19</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="8"/>
-      <c r="J16" s="16"/>
+      <c r="J16" s="33"/>
       <c r="K16" s="9"/>
     </row>
     <row r="17" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="48"/>
-      <c r="B17" s="65" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="34" t="s">
+      <c r="A17" s="62"/>
+      <c r="B17" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="49">
+      <c r="D17" s="24">
         <v>2019</v>
       </c>
-      <c r="E17" s="49" t="s">
+      <c r="E17" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="49">
-        <v>2</v>
-      </c>
-      <c r="G17" s="50" t="s">
+      <c r="F17" s="24">
+        <v>2</v>
+      </c>
+      <c r="G17" s="25" t="s">
         <v>19</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="8"/>
-      <c r="J17" s="16" t="s">
+      <c r="J17" s="33" t="s">
         <v>4</v>
       </c>
       <c r="K17" s="9" t="s">
@@ -1715,78 +1715,78 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="48"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="32">
+      <c r="A18" s="62"/>
+      <c r="B18" s="46"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="20">
         <v>2018</v>
       </c>
-      <c r="E18" s="32" t="s">
+      <c r="E18" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="F18" s="32">
-        <v>2</v>
-      </c>
-      <c r="G18" s="33" t="s">
+      <c r="F18" s="20">
+        <v>2</v>
+      </c>
+      <c r="G18" s="21" t="s">
         <v>26</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="8"/>
-      <c r="J18" s="16"/>
+      <c r="J18" s="33"/>
       <c r="K18" s="9" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="59"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="36">
+      <c r="A19" s="63"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="60"/>
+      <c r="D19" s="22">
         <v>2021</v>
       </c>
-      <c r="E19" s="36" t="s">
+      <c r="E19" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="F19" s="36">
-        <v>2</v>
-      </c>
-      <c r="G19" s="37" t="s">
+      <c r="F19" s="22">
+        <v>2</v>
+      </c>
+      <c r="G19" s="23" t="s">
         <v>21</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="10"/>
-      <c r="J19" s="17"/>
+      <c r="J19" s="34"/>
       <c r="K19" s="11" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="51" t="s">
+      <c r="A20" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" s="22" t="s">
+      <c r="B20" s="53" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="22">
+      <c r="D20" s="12">
         <v>2022</v>
       </c>
-      <c r="E20" s="22" t="s">
+      <c r="E20" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F20" s="22">
-        <v>2</v>
-      </c>
-      <c r="G20" s="23" t="s">
+      <c r="F20" s="12">
+        <v>2</v>
+      </c>
+      <c r="G20" s="13" t="s">
         <v>70</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J20" s="15" t="s">
+      <c r="J20" s="35" t="s">
         <v>2</v>
       </c>
       <c r="K20" s="7" t="s">
@@ -1794,228 +1794,228 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="52"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="24" t="s">
+      <c r="A21" s="51"/>
+      <c r="B21" s="54"/>
+      <c r="C21" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="24">
+      <c r="D21" s="14">
         <v>2019</v>
       </c>
-      <c r="E21" s="24" t="s">
+      <c r="E21" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F21" s="24">
-        <v>4</v>
-      </c>
-      <c r="G21" s="25" t="s">
+      <c r="F21" s="14">
+        <v>4</v>
+      </c>
+      <c r="G21" s="15" t="s">
         <v>19</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="8"/>
-      <c r="J21" s="16"/>
+      <c r="J21" s="33"/>
       <c r="K21" s="9" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="52"/>
-      <c r="B22" s="60"/>
-      <c r="C22" s="57" t="s">
+      <c r="A22" s="51"/>
+      <c r="B22" s="64"/>
+      <c r="C22" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="57">
+      <c r="D22" s="28">
         <v>2019</v>
       </c>
-      <c r="E22" s="57" t="s">
-        <v>20</v>
-      </c>
-      <c r="F22" s="57">
-        <v>4</v>
-      </c>
-      <c r="G22" s="58" t="s">
+      <c r="E22" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="28">
+        <v>4</v>
+      </c>
+      <c r="G22" s="29" t="s">
         <v>26</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="8"/>
-      <c r="J22" s="16"/>
+      <c r="J22" s="33"/>
       <c r="K22" s="9" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="52"/>
-      <c r="B23" s="12" t="s">
+      <c r="A23" s="51"/>
+      <c r="B23" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="22">
+      <c r="D23" s="12">
         <v>2015</v>
       </c>
-      <c r="E23" s="22" t="s">
+      <c r="E23" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="22">
-        <v>4</v>
-      </c>
-      <c r="G23" s="23" t="s">
+      <c r="F23" s="12">
+        <v>4</v>
+      </c>
+      <c r="G23" s="13" t="s">
         <v>19</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="8"/>
-      <c r="J23" s="16" t="s">
+      <c r="J23" s="33" t="s">
         <v>3</v>
       </c>
       <c r="K23" s="9"/>
     </row>
     <row r="24" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="52"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="24" t="s">
+      <c r="A24" s="51"/>
+      <c r="B24" s="54"/>
+      <c r="C24" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="24">
+      <c r="D24" s="14">
         <v>2019</v>
       </c>
-      <c r="E24" s="24" t="s">
+      <c r="E24" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F24" s="24">
-        <v>2</v>
-      </c>
-      <c r="G24" s="25" t="s">
+      <c r="F24" s="14">
+        <v>2</v>
+      </c>
+      <c r="G24" s="15" t="s">
         <v>26</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="8"/>
-      <c r="J24" s="16"/>
+      <c r="J24" s="33"/>
       <c r="K24" s="9"/>
     </row>
     <row r="25" spans="1:11" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="52"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="28" t="s">
+      <c r="A25" s="51"/>
+      <c r="B25" s="55"/>
+      <c r="C25" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="28">
+      <c r="D25" s="16">
         <v>2018</v>
       </c>
-      <c r="E25" s="28" t="s">
+      <c r="E25" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F25" s="28">
-        <v>4</v>
-      </c>
-      <c r="G25" s="29" t="s">
+      <c r="F25" s="16">
+        <v>4</v>
+      </c>
+      <c r="G25" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="8"/>
-      <c r="J25" s="16"/>
+      <c r="J25" s="33"/>
       <c r="K25" s="9"/>
     </row>
     <row r="26" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="52"/>
-      <c r="B26" s="61" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="53">
+      <c r="A26" s="51"/>
+      <c r="B26" s="65" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="26">
         <v>86</v>
       </c>
-      <c r="D26" s="53">
+      <c r="D26" s="26">
         <v>2019</v>
       </c>
-      <c r="E26" s="53" t="s">
+      <c r="E26" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="F26" s="53">
-        <v>2</v>
-      </c>
-      <c r="G26" s="54" t="s">
+      <c r="F26" s="26">
+        <v>2</v>
+      </c>
+      <c r="G26" s="27" t="s">
         <v>21</v>
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="8"/>
-      <c r="J26" s="16" t="s">
+      <c r="J26" s="33" t="s">
         <v>4</v>
       </c>
       <c r="K26" s="9"/>
     </row>
     <row r="27" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="52"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="24" t="s">
+      <c r="A27" s="51"/>
+      <c r="B27" s="54"/>
+      <c r="C27" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="24">
+      <c r="D27" s="14">
         <v>2022</v>
       </c>
-      <c r="E27" s="24" t="s">
+      <c r="E27" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F27" s="24">
-        <v>2</v>
-      </c>
-      <c r="G27" s="25" t="s">
+      <c r="F27" s="14">
+        <v>2</v>
+      </c>
+      <c r="G27" s="15" t="s">
         <v>19</v>
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="8"/>
-      <c r="J27" s="16"/>
+      <c r="J27" s="33"/>
       <c r="K27" s="9"/>
     </row>
     <row r="28" spans="1:11" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="56"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="28" t="s">
+      <c r="A28" s="52"/>
+      <c r="B28" s="55"/>
+      <c r="C28" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D28" s="28">
+      <c r="D28" s="16">
         <v>2023</v>
       </c>
-      <c r="E28" s="28" t="s">
+      <c r="E28" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="F28" s="28">
-        <v>2</v>
-      </c>
-      <c r="G28" s="29" t="s">
+      <c r="F28" s="16">
+        <v>2</v>
+      </c>
+      <c r="G28" s="17" t="s">
         <v>26</v>
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="10"/>
-      <c r="J28" s="17"/>
+      <c r="J28" s="34"/>
       <c r="K28" s="11"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="47" t="s">
+      <c r="A29" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="C29" s="38" t="s">
+      <c r="B29" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="D29" s="30">
+      <c r="D29" s="18">
         <v>2019</v>
       </c>
-      <c r="E29" s="30" t="s">
+      <c r="E29" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="F29" s="30">
-        <v>4</v>
-      </c>
-      <c r="G29" s="31" t="s">
+      <c r="F29" s="18">
+        <v>4</v>
+      </c>
+      <c r="G29" s="19" t="s">
         <v>21</v>
       </c>
       <c r="H29" s="2"/>
       <c r="I29" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J29" s="15" t="s">
+      <c r="J29" s="35" t="s">
         <v>2</v>
       </c>
       <c r="K29" s="7" t="s">
@@ -2023,216 +2023,216 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="48"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="32">
+      <c r="A30" s="62"/>
+      <c r="B30" s="46"/>
+      <c r="C30" s="59"/>
+      <c r="D30" s="20">
         <v>2020</v>
       </c>
-      <c r="E30" s="32" t="s">
+      <c r="E30" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="F30" s="32">
-        <v>4</v>
-      </c>
-      <c r="G30" s="33" t="s">
+      <c r="F30" s="20">
+        <v>4</v>
+      </c>
+      <c r="G30" s="21" t="s">
         <v>19</v>
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="8"/>
-      <c r="J30" s="16"/>
+      <c r="J30" s="33"/>
       <c r="K30" s="9" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="48"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="35"/>
-      <c r="D31" s="36">
+      <c r="A31" s="62"/>
+      <c r="B31" s="48"/>
+      <c r="C31" s="60"/>
+      <c r="D31" s="22">
         <v>2021</v>
       </c>
-      <c r="E31" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="F31" s="36">
-        <v>4</v>
-      </c>
-      <c r="G31" s="37" t="s">
+      <c r="E31" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" s="22">
+        <v>4</v>
+      </c>
+      <c r="G31" s="23" t="s">
         <v>26</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="8"/>
-      <c r="J31" s="16"/>
+      <c r="J31" s="33"/>
       <c r="K31" s="9" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="48"/>
-      <c r="B32" s="19" t="s">
+      <c r="A32" s="62"/>
+      <c r="B32" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="C32" s="30" t="s">
+      <c r="C32" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D32" s="30">
+      <c r="D32" s="18">
         <v>2019</v>
       </c>
-      <c r="E32" s="30" t="s">
+      <c r="E32" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="F32" s="30">
-        <v>4</v>
-      </c>
-      <c r="G32" s="31" t="s">
+      <c r="F32" s="18">
+        <v>4</v>
+      </c>
+      <c r="G32" s="19" t="s">
         <v>26</v>
       </c>
       <c r="H32" s="2"/>
       <c r="I32" s="8"/>
-      <c r="J32" s="16" t="s">
+      <c r="J32" s="33" t="s">
         <v>3</v>
       </c>
       <c r="K32" s="9"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="48"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="32" t="s">
+      <c r="A33" s="62"/>
+      <c r="B33" s="46"/>
+      <c r="C33" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="D33" s="32">
+      <c r="D33" s="20">
         <v>2020</v>
       </c>
-      <c r="E33" s="32" t="s">
+      <c r="E33" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="F33" s="32">
-        <v>2</v>
-      </c>
-      <c r="G33" s="33" t="s">
+      <c r="F33" s="20">
+        <v>2</v>
+      </c>
+      <c r="G33" s="21" t="s">
         <v>19</v>
       </c>
       <c r="H33" s="2"/>
       <c r="I33" s="8"/>
-      <c r="J33" s="16"/>
+      <c r="J33" s="33"/>
       <c r="K33" s="9"/>
     </row>
     <row r="34" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="48"/>
-      <c r="B34" s="21"/>
-      <c r="C34" s="36" t="s">
+      <c r="A34" s="62"/>
+      <c r="B34" s="48"/>
+      <c r="C34" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="D34" s="36">
+      <c r="D34" s="22">
         <v>2019</v>
       </c>
-      <c r="E34" s="36" t="s">
+      <c r="E34" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="F34" s="36">
-        <v>4</v>
-      </c>
-      <c r="G34" s="37" t="s">
+      <c r="F34" s="22">
+        <v>4</v>
+      </c>
+      <c r="G34" s="23" t="s">
         <v>21</v>
       </c>
       <c r="H34" s="2"/>
       <c r="I34" s="8"/>
-      <c r="J34" s="16"/>
+      <c r="J34" s="33"/>
       <c r="K34" s="9"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="48"/>
-      <c r="B35" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35" s="30" t="s">
+      <c r="A35" s="62"/>
+      <c r="B35" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="30">
+      <c r="D35" s="18">
         <v>2015</v>
       </c>
-      <c r="E35" s="30" t="s">
+      <c r="E35" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="F35" s="30">
-        <v>2</v>
-      </c>
-      <c r="G35" s="31" t="s">
+      <c r="F35" s="18">
+        <v>2</v>
+      </c>
+      <c r="G35" s="19" t="s">
         <v>21</v>
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="8"/>
-      <c r="J35" s="16" t="s">
+      <c r="J35" s="33" t="s">
         <v>4</v>
       </c>
       <c r="K35" s="9"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="48"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="32" t="s">
+      <c r="A36" s="62"/>
+      <c r="B36" s="46"/>
+      <c r="C36" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="D36" s="32">
+      <c r="D36" s="20">
         <v>2015</v>
       </c>
-      <c r="E36" s="32" t="s">
+      <c r="E36" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="F36" s="32">
-        <v>2</v>
-      </c>
-      <c r="G36" s="33" t="s">
+      <c r="F36" s="20">
+        <v>2</v>
+      </c>
+      <c r="G36" s="21" t="s">
         <v>19</v>
       </c>
       <c r="H36" s="2"/>
       <c r="I36" s="8"/>
-      <c r="J36" s="16"/>
+      <c r="J36" s="33"/>
       <c r="K36" s="9"/>
     </row>
     <row r="37" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="59"/>
-      <c r="B37" s="21"/>
-      <c r="C37" s="36" t="s">
+      <c r="A37" s="63"/>
+      <c r="B37" s="48"/>
+      <c r="C37" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="D37" s="36">
+      <c r="D37" s="22">
         <v>2013</v>
       </c>
-      <c r="E37" s="36" t="s">
+      <c r="E37" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="F37" s="36">
-        <v>2</v>
-      </c>
-      <c r="G37" s="37" t="s">
+      <c r="F37" s="22">
+        <v>2</v>
+      </c>
+      <c r="G37" s="23" t="s">
         <v>69</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="10"/>
-      <c r="J37" s="17"/>
+      <c r="J37" s="34"/>
       <c r="K37" s="11"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="51" t="s">
+      <c r="A38" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C38" s="39" t="s">
+      <c r="B38" s="53" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="D38" s="40"/>
-      <c r="E38" s="40"/>
-      <c r="F38" s="40"/>
-      <c r="G38" s="41"/>
+      <c r="D38" s="37"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="37"/>
+      <c r="G38" s="38"/>
       <c r="H38" s="2"/>
       <c r="I38" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="J38" s="15" t="s">
+      <c r="J38" s="35" t="s">
         <v>2</v>
       </c>
       <c r="K38" s="9" t="s">
@@ -2240,54 +2240,54 @@
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="52"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="42"/>
-      <c r="D39" s="55"/>
-      <c r="E39" s="55"/>
-      <c r="F39" s="55"/>
-      <c r="G39" s="43"/>
+      <c r="A39" s="51"/>
+      <c r="B39" s="54"/>
+      <c r="C39" s="39"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="40"/>
+      <c r="F39" s="40"/>
+      <c r="G39" s="41"/>
       <c r="H39" s="2"/>
       <c r="I39" s="8"/>
-      <c r="J39" s="16"/>
+      <c r="J39" s="33"/>
       <c r="K39" s="9"/>
     </row>
     <row r="40" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="52"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="44"/>
-      <c r="D40" s="45"/>
-      <c r="E40" s="45"/>
-      <c r="F40" s="45"/>
-      <c r="G40" s="46"/>
+      <c r="A40" s="51"/>
+      <c r="B40" s="55"/>
+      <c r="C40" s="42"/>
+      <c r="D40" s="43"/>
+      <c r="E40" s="43"/>
+      <c r="F40" s="43"/>
+      <c r="G40" s="44"/>
       <c r="H40" s="2"/>
       <c r="I40" s="8"/>
-      <c r="J40" s="16"/>
+      <c r="J40" s="33"/>
       <c r="K40" s="9"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="52"/>
-      <c r="B41" s="12" t="s">
+      <c r="A41" s="51"/>
+      <c r="B41" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="C41" s="22" t="s">
+      <c r="C41" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="D41" s="22">
+      <c r="D41" s="12">
         <v>2023</v>
       </c>
-      <c r="E41" s="22" t="s">
+      <c r="E41" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="F41" s="22">
-        <v>4</v>
-      </c>
-      <c r="G41" s="23" t="s">
+      <c r="F41" s="12">
+        <v>4</v>
+      </c>
+      <c r="G41" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H41" s="2"/>
       <c r="I41" s="8"/>
-      <c r="J41" s="16" t="s">
+      <c r="J41" s="33" t="s">
         <v>3</v>
       </c>
       <c r="K41" s="9" t="s">
@@ -2295,70 +2295,70 @@
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="52"/>
-      <c r="B42" s="13"/>
-      <c r="C42" s="24" t="s">
+      <c r="A42" s="51"/>
+      <c r="B42" s="54"/>
+      <c r="C42" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="D42" s="24">
+      <c r="D42" s="14">
         <v>2019</v>
       </c>
-      <c r="E42" s="24" t="s">
+      <c r="E42" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F42" s="24">
-        <v>4</v>
-      </c>
-      <c r="G42" s="25" t="s">
+      <c r="F42" s="14">
+        <v>4</v>
+      </c>
+      <c r="G42" s="15" t="s">
         <v>19</v>
       </c>
       <c r="H42" s="2"/>
       <c r="I42" s="8"/>
-      <c r="J42" s="16"/>
+      <c r="J42" s="33"/>
       <c r="K42" s="9" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="52"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="28" t="s">
+      <c r="A43" s="51"/>
+      <c r="B43" s="55"/>
+      <c r="C43" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="D43" s="28">
+      <c r="D43" s="16">
         <v>2018</v>
       </c>
-      <c r="E43" s="28" t="s">
+      <c r="E43" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F43" s="28">
-        <v>4</v>
-      </c>
-      <c r="G43" s="29" t="s">
+      <c r="F43" s="16">
+        <v>4</v>
+      </c>
+      <c r="G43" s="17" t="s">
         <v>69</v>
       </c>
       <c r="H43" s="2"/>
       <c r="I43" s="8"/>
-      <c r="J43" s="16"/>
+      <c r="J43" s="33"/>
       <c r="K43" s="9" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="52"/>
-      <c r="B44" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C44" s="39" t="s">
+      <c r="A44" s="51"/>
+      <c r="B44" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="D44" s="40"/>
-      <c r="E44" s="40"/>
-      <c r="F44" s="40"/>
-      <c r="G44" s="41"/>
+      <c r="D44" s="37"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="37"/>
+      <c r="G44" s="38"/>
       <c r="H44" s="2"/>
       <c r="I44" s="8"/>
-      <c r="J44" s="16" t="s">
+      <c r="J44" s="33" t="s">
         <v>4</v>
       </c>
       <c r="K44" s="9" t="s">
@@ -2366,29 +2366,29 @@
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="52"/>
-      <c r="B45" s="13"/>
-      <c r="C45" s="42"/>
-      <c r="D45" s="55"/>
-      <c r="E45" s="55"/>
-      <c r="F45" s="55"/>
-      <c r="G45" s="43"/>
+      <c r="A45" s="51"/>
+      <c r="B45" s="54"/>
+      <c r="C45" s="39"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="41"/>
       <c r="H45" s="2"/>
       <c r="I45" s="8"/>
-      <c r="J45" s="16"/>
+      <c r="J45" s="33"/>
       <c r="K45" s="9"/>
     </row>
     <row r="46" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="56"/>
-      <c r="B46" s="14"/>
-      <c r="C46" s="44"/>
-      <c r="D46" s="45"/>
-      <c r="E46" s="45"/>
-      <c r="F46" s="45"/>
-      <c r="G46" s="46"/>
+      <c r="A46" s="52"/>
+      <c r="B46" s="55"/>
+      <c r="C46" s="42"/>
+      <c r="D46" s="43"/>
+      <c r="E46" s="43"/>
+      <c r="F46" s="43"/>
+      <c r="G46" s="44"/>
       <c r="H46" s="2"/>
       <c r="I46" s="10"/>
-      <c r="J46" s="17"/>
+      <c r="J46" s="34"/>
       <c r="K46" s="11"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -2404,39 +2404,14 @@
       <c r="C49" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D49" s="18" t="s">
+      <c r="D49" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="E49" s="18"/>
-      <c r="F49" s="18"/>
+      <c r="E49" s="32"/>
+      <c r="F49" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="J32:J34"/>
-    <mergeCell ref="J35:J37"/>
-    <mergeCell ref="J38:J40"/>
-    <mergeCell ref="J41:J43"/>
-    <mergeCell ref="J44:J46"/>
-    <mergeCell ref="C38:G40"/>
-    <mergeCell ref="C44:G46"/>
-    <mergeCell ref="J2:J4"/>
-    <mergeCell ref="J5:J7"/>
-    <mergeCell ref="J8:J10"/>
-    <mergeCell ref="J11:J13"/>
-    <mergeCell ref="J14:J16"/>
-    <mergeCell ref="J17:J19"/>
-    <mergeCell ref="J20:J22"/>
-    <mergeCell ref="J23:J25"/>
-    <mergeCell ref="J26:J28"/>
-    <mergeCell ref="J29:J31"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="A38:A46"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="B44:B46"/>
     <mergeCell ref="C8:C10"/>
     <mergeCell ref="C29:C31"/>
     <mergeCell ref="C17:C19"/>
@@ -2453,6 +2428,31 @@
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="A11:A19"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="A38:A46"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="J17:J19"/>
+    <mergeCell ref="J20:J22"/>
+    <mergeCell ref="J23:J25"/>
+    <mergeCell ref="J26:J28"/>
+    <mergeCell ref="J29:J31"/>
+    <mergeCell ref="J2:J4"/>
+    <mergeCell ref="J5:J7"/>
+    <mergeCell ref="J8:J10"/>
+    <mergeCell ref="J11:J13"/>
+    <mergeCell ref="J14:J16"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="J32:J34"/>
+    <mergeCell ref="J35:J37"/>
+    <mergeCell ref="J38:J40"/>
+    <mergeCell ref="J41:J43"/>
+    <mergeCell ref="J44:J46"/>
+    <mergeCell ref="C38:G40"/>
+    <mergeCell ref="C44:G46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>